<commit_message>
Read table content from Excel finished
</commit_message>
<xml_diff>
--- a/src/VerySimpleDashboard.Tests/Excel Importer/Test Document 2.xlsx
+++ b/src/VerySimpleDashboard.Tests/Excel Importer/Test Document 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Internet connection speed" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="404">
   <si>
     <t>Country/Territory</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Belgium</t>
-  </si>
-  <si>
-    <t>9.8</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -1623,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1658,9 +1655,6 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1670,25 +1664,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1696,423 +1682,423 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
         <v>51</v>
-      </c>
-      <c r="B29" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
         <v>53</v>
-      </c>
-      <c r="B30" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
         <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
         <v>58</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
         <v>60</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
         <v>62</v>
-      </c>
-      <c r="B35" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
         <v>64</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
         <v>66</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
         <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
         <v>71</v>
-      </c>
-      <c r="B40" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
         <v>73</v>
-      </c>
-      <c r="B41" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
         <v>75</v>
-      </c>
-      <c r="B42" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
         <v>79</v>
-      </c>
-      <c r="B45" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" t="s">
         <v>82</v>
-      </c>
-      <c r="B47" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
         <v>84</v>
-      </c>
-      <c r="B48" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
         <v>87</v>
-      </c>
-      <c r="B50" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
         <v>89</v>
-      </c>
-      <c r="B51" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
         <v>91</v>
-      </c>
-      <c r="B52" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" t="s">
         <v>94</v>
-      </c>
-      <c r="B55" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" t="s">
         <v>96</v>
-      </c>
-      <c r="B56" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" t="s">
         <v>98</v>
-      </c>
-      <c r="B57" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" t="s">
         <v>100</v>
-      </c>
-      <c r="B58" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" t="s">
         <v>102</v>
-      </c>
-      <c r="B59" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" t="s">
         <v>104</v>
-      </c>
-      <c r="B60" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
         <v>2</v>
@@ -2120,18 +2106,18 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2143,7 +2129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -2158,27 +2144,27 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>403</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4">
         <v>1659269</v>
@@ -2187,7 +2173,7 @@
         <v>99</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E2" t="b">
         <f>B2&gt;1000000</f>
@@ -2211,7 +2197,7 @@
         <v>100</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E3" t="b">
         <f t="shared" ref="E3:E58" si="0">B3&gt;1000000</f>
@@ -2224,7 +2210,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="4">
         <v>5690291</v>
@@ -2233,7 +2219,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E4" t="b">
         <f t="shared" si="0"/>
@@ -2246,7 +2232,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="6">
         <v>7354</v>
@@ -2255,7 +2241,7 @@
         <v>175</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E5" t="b">
         <f t="shared" si="0"/>
@@ -2268,7 +2254,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="4">
         <v>3058195</v>
@@ -2277,7 +2263,7 @@
         <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E6" t="b">
         <f t="shared" si="0"/>
@@ -2297,7 +2283,7 @@
         <v>204</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E7" t="b">
         <f t="shared" si="0"/>
@@ -2310,7 +2296,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="4">
         <v>74586</v>
@@ -2319,7 +2305,7 @@
         <v>174</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E8" t="b">
         <f t="shared" si="0"/>
@@ -2341,7 +2327,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E9" t="b">
         <f t="shared" si="0"/>
@@ -2354,14 +2340,14 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3">
         <v>112</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E10" t="b">
         <f t="shared" si="0"/>
@@ -2374,7 +2360,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="6">
         <v>7965</v>
@@ -2383,7 +2369,7 @@
         <v>172</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E11" t="b">
         <f t="shared" si="0"/>
@@ -2403,7 +2389,7 @@
         <v>212</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E12" t="b">
         <f t="shared" si="0"/>
@@ -2423,7 +2409,7 @@
         <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E13" t="b">
         <f t="shared" si="0"/>
@@ -2443,7 +2429,7 @@
         <v>50</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E14" t="b">
         <f t="shared" si="0"/>
@@ -2463,7 +2449,7 @@
         <v>59</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E15" t="b">
         <f t="shared" si="0"/>
@@ -2476,7 +2462,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="4">
         <v>1098546</v>
@@ -2485,7 +2471,7 @@
         <v>117</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E16" t="b">
         <f t="shared" si="0"/>
@@ -2507,7 +2493,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E17" t="b">
         <f t="shared" si="0"/>
@@ -2520,7 +2506,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="4">
         <v>210994</v>
@@ -2529,7 +2515,7 @@
         <v>153</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E18" t="b">
         <f t="shared" si="0"/>
@@ -2549,7 +2535,7 @@
         <v>63</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E19" t="b">
         <f t="shared" si="0"/>
@@ -2571,7 +2557,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E20" t="b">
         <f t="shared" si="0"/>
@@ -2584,7 +2570,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="6">
         <v>8193</v>
@@ -2593,7 +2579,7 @@
         <v>171</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E21" t="b">
         <f t="shared" si="0"/>
@@ -2606,7 +2592,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" s="4">
         <v>364534</v>
@@ -2615,7 +2601,7 @@
         <v>136</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E22" t="b">
         <f t="shared" si="0"/>
@@ -2628,7 +2614,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" s="6">
         <v>6307</v>
@@ -2637,7 +2623,7 @@
         <v>178</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E23" t="b">
         <f t="shared" si="0"/>
@@ -2650,7 +2636,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="4">
         <v>182338</v>
@@ -2659,7 +2645,7 @@
         <v>155</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E24" t="b">
         <f t="shared" si="0"/>
@@ -2672,7 +2658,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" s="6">
         <v>3517991</v>
@@ -2681,7 +2667,7 @@
         <v>75</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E25" t="b">
         <f t="shared" si="0"/>
@@ -2694,7 +2680,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" s="4">
         <v>2535356</v>
@@ -2703,7 +2689,7 @@
         <v>83</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E26" t="b">
         <f t="shared" si="0"/>
@@ -2716,7 +2702,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="6">
         <v>241272</v>
@@ -2725,7 +2711,7 @@
         <v>148</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E27" t="b">
         <f t="shared" si="0"/>
@@ -2738,7 +2724,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="4">
         <v>99357737</v>
@@ -2747,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E28" t="b">
         <f t="shared" si="0"/>
@@ -2760,7 +2746,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29" s="6">
         <v>246388</v>
@@ -2769,7 +2755,7 @@
         <v>147</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E29" t="b">
         <f t="shared" si="0"/>
@@ -2782,7 +2768,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="4">
         <v>3881287</v>
@@ -2791,7 +2777,7 @@
         <v>72</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E30" t="b">
         <f t="shared" si="0"/>
@@ -2818,7 +2804,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" s="6">
         <v>128799</v>
@@ -2827,7 +2813,7 @@
         <v>167</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E33" t="b">
         <f t="shared" si="0"/>
@@ -2840,7 +2826,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B34" s="4">
         <v>738641</v>
@@ -2849,7 +2835,7 @@
         <v>122</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" t="b">
         <f t="shared" si="0"/>
@@ -2869,7 +2855,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="4">
         <v>29760764</v>
@@ -2878,7 +2864,7 @@
         <v>20</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E36" t="b">
         <f t="shared" si="0"/>
@@ -2891,7 +2877,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" s="6">
         <v>181905</v>
@@ -2900,7 +2886,7 @@
         <v>156</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E37" t="b">
         <f t="shared" si="0"/>
@@ -2913,7 +2899,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B38" s="4">
         <v>38961</v>
@@ -2922,7 +2908,7 @@
         <v>191</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E38" t="b">
         <f t="shared" si="0"/>
@@ -2935,7 +2921,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" s="6">
         <v>151716</v>
@@ -2944,7 +2930,7 @@
         <v>160</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" t="b">
         <f t="shared" si="0"/>
@@ -2964,7 +2950,7 @@
         <v>149</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E40" t="b">
         <f t="shared" si="0"/>
@@ -2984,7 +2970,7 @@
         <v>39</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E41" t="b">
         <f t="shared" si="0"/>
@@ -3004,7 +2990,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E42" t="b">
         <f t="shared" si="0"/>
@@ -3024,7 +3010,7 @@
         <v>23</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E43" t="b">
         <f t="shared" si="0"/>
@@ -3044,7 +3030,7 @@
         <v>183</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" t="b">
         <f t="shared" si="0"/>
@@ -3064,7 +3050,7 @@
         <v>88</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E45" t="b">
         <f t="shared" si="0"/>
@@ -3077,7 +3063,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" s="4">
         <v>2822427</v>
@@ -3086,7 +3072,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E46" t="b">
         <f t="shared" si="0"/>
@@ -3099,7 +3085,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="6">
         <v>2839881</v>
@@ -3108,7 +3094,7 @@
         <v>79</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E47" t="b">
         <f t="shared" si="0"/>
@@ -3121,7 +3107,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B48" s="4">
         <v>694223</v>
@@ -3130,7 +3116,7 @@
         <v>126</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E48" t="b">
         <f t="shared" si="0"/>
@@ -3143,7 +3129,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" s="6">
         <v>7632975</v>
@@ -3152,7 +3138,7 @@
         <v>45</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E49" t="b">
         <f t="shared" si="0"/>
@@ -3165,7 +3151,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B50" s="4">
         <v>1236438</v>
@@ -3174,7 +3160,7 @@
         <v>110</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E50" t="b">
         <f t="shared" si="0"/>
@@ -3187,7 +3173,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51" s="6">
         <v>5155411</v>
@@ -3196,7 +3182,7 @@
         <v>58</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E51" t="b">
         <f t="shared" si="0"/>
@@ -3209,7 +3195,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B52" s="4">
         <v>64021</v>
@@ -3218,7 +3204,7 @@
         <v>177</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E52" t="b">
         <f t="shared" si="0"/>
@@ -3231,7 +3217,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" s="6">
         <v>40349</v>
@@ -3240,7 +3226,7 @@
         <v>188</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E53" t="b">
         <f t="shared" si="0"/>
@@ -3253,7 +3239,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="4">
         <v>4539869</v>
@@ -3262,7 +3248,7 @@
         <v>62</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E54" t="b">
         <f t="shared" si="0"/>
@@ -3275,7 +3261,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" s="6">
         <v>10461</v>
@@ -3284,7 +3270,7 @@
         <v>203</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E55" t="b">
         <f t="shared" si="0"/>
@@ -3297,7 +3283,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B56" s="4">
         <v>5348765</v>
@@ -3306,7 +3292,7 @@
         <v>56</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E56" t="b">
         <f t="shared" si="0"/>
@@ -3319,7 +3305,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" s="6">
         <v>36881374</v>
@@ -3328,7 +3314,7 @@
         <v>15</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E57" t="b">
         <f t="shared" si="0"/>
@@ -3341,7 +3327,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B58" s="4">
         <v>1553115</v>
@@ -3350,7 +3336,7 @@
         <v>104</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E58" t="b">
         <f t="shared" si="0"/>
@@ -3440,7 +3426,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B70" s="4">
         <v>2079917</v>
@@ -3449,7 +3435,7 @@
         <v>91</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E70" t="b">
         <f t="shared" ref="E70:E130" si="2">B70&gt;1000000</f>
@@ -3462,7 +3448,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B71" s="6">
         <v>68296919</v>
@@ -3471,7 +3457,7 @@
         <v>7</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E71" t="b">
         <f t="shared" si="2"/>
@@ -3484,7 +3470,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B72" s="4">
         <v>4217454</v>
@@ -3493,7 +3479,7 @@
         <v>69</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E72" t="b">
         <f t="shared" si="2"/>
@@ -3506,7 +3492,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B73" s="6">
         <v>18877</v>
@@ -3515,7 +3501,7 @@
         <v>200</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E73" t="b">
         <f t="shared" si="2"/>
@@ -3528,7 +3514,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B74" s="4">
         <v>6029983</v>
@@ -3537,7 +3523,7 @@
         <v>52</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E74" t="b">
         <f t="shared" si="2"/>
@@ -3550,7 +3536,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B75" s="6">
         <v>37442</v>
@@ -3559,7 +3545,7 @@
         <v>193</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E75" t="b">
         <f t="shared" si="2"/>
@@ -3572,7 +3558,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B76" s="4">
         <v>45883</v>
@@ -3581,7 +3567,7 @@
         <v>182</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E76" t="b">
         <f t="shared" si="2"/>
@@ -3594,7 +3580,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B77" s="6">
         <v>98402</v>
@@ -3603,7 +3589,7 @@
         <v>168</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E77" t="b">
         <f t="shared" si="2"/>
@@ -3616,7 +3602,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B78" s="4">
         <v>2255845</v>
@@ -3625,7 +3611,7 @@
         <v>86</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E78" t="b">
         <f t="shared" si="2"/>
@@ -3638,7 +3624,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B79" s="6">
         <v>162202</v>
@@ -3647,7 +3633,7 @@
         <v>158</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E79" t="b">
         <f t="shared" si="2"/>
@@ -3660,7 +3646,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B80" s="4">
         <v>47132</v>
@@ -3669,7 +3655,7 @@
         <v>181</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E80" t="b">
         <f t="shared" si="2"/>
@@ -3682,7 +3668,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B81" s="6">
         <v>254534</v>
@@ -3691,7 +3677,7 @@
         <v>146</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E81" t="b">
         <f t="shared" si="2"/>
@@ -3704,7 +3690,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B82" s="4">
         <v>1065470</v>
@@ -3713,7 +3699,7 @@
         <v>118</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E82" t="b">
         <f t="shared" si="2"/>
@@ -3726,7 +3712,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B83" s="6">
         <v>1503350</v>
@@ -3735,7 +3721,7 @@
         <v>105</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E83" t="b">
         <f t="shared" si="2"/>
@@ -3748,7 +3734,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B84" s="4">
         <v>5207762</v>
@@ -3757,7 +3743,7 @@
         <v>57</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E84" t="b">
         <f t="shared" si="2"/>
@@ -3770,7 +3756,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B85" s="6">
         <v>7170086</v>
@@ -3779,7 +3765,7 @@
         <v>47</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E85" t="b">
         <f t="shared" si="2"/>
@@ -3792,7 +3778,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B86" s="4">
         <v>300656</v>
@@ -3801,7 +3787,7 @@
         <v>139</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E86" t="b">
         <f t="shared" si="2"/>
@@ -3814,7 +3800,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B87" s="6">
         <v>151598994</v>
@@ -3823,7 +3809,7 @@
         <v>3</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E87" t="b">
         <f t="shared" si="2"/>
@@ -3836,7 +3822,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B88" s="4">
         <v>38191873</v>
@@ -3845,7 +3831,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E88" t="b">
         <f t="shared" si="2"/>
@@ -3858,7 +3844,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B89" s="6">
         <v>20504000</v>
@@ -3867,7 +3853,7 @@
         <v>24</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E89" t="b">
         <f t="shared" si="2"/>
@@ -3880,7 +3866,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B90" s="4">
         <v>2210175</v>
@@ -3889,7 +3875,7 @@
         <v>87</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E90" t="b">
         <f t="shared" si="2"/>
@@ -3902,7 +3888,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B91" s="6">
         <v>3730402</v>
@@ -3911,7 +3897,7 @@
         <v>74</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E91" t="b">
         <f t="shared" si="2"/>
@@ -3924,7 +3910,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B92" s="4">
         <v>5568961</v>
@@ -3933,7 +3919,7 @@
         <v>54</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E92" t="b">
         <f t="shared" si="2"/>
@@ -3946,7 +3932,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B93" s="6">
         <v>35531527</v>
@@ -3955,7 +3941,7 @@
         <v>18</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E93" t="b">
         <f t="shared" si="2"/>
@@ -3968,7 +3954,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B94" s="4">
         <v>522231</v>
@@ -3977,7 +3963,7 @@
         <v>130</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E94" t="b">
         <f t="shared" si="2"/>
@@ -3990,7 +3976,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B95" s="6">
         <v>1343472</v>
@@ -3999,7 +3985,7 @@
         <v>108</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E95" t="b">
         <f t="shared" si="2"/>
@@ -4012,7 +3998,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B96" s="4">
         <v>100684474</v>
@@ -4021,7 +4007,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E96" t="b">
         <f t="shared" si="2"/>
@@ -4034,7 +4020,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B97" s="6">
         <v>38958</v>
@@ -4043,7 +4029,7 @@
         <v>192</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E97" t="b">
         <f t="shared" si="2"/>
@@ -4056,7 +4042,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B98" s="4">
         <v>2668644</v>
@@ -4065,7 +4051,7 @@
         <v>81</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E98" t="b">
         <f t="shared" si="2"/>
@@ -4078,7 +4064,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B99" s="6">
         <v>9341977</v>
@@ -4087,7 +4073,7 @@
         <v>42</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E99" t="b">
         <f t="shared" si="2"/>
@@ -4100,7 +4086,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B100" s="4">
         <v>13805311</v>
@@ -4109,7 +4095,7 @@
         <v>35</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E100" t="b">
         <f t="shared" si="2"/>
@@ -4122,7 +4108,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B101" s="6">
         <v>10962</v>
@@ -4131,7 +4117,7 @@
         <v>202</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E101" t="b">
         <f t="shared" si="2"/>
@@ -4144,7 +4130,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B102" s="4">
         <v>2095304</v>
@@ -4153,7 +4139,7 @@
         <v>90</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E102" t="b">
         <f t="shared" si="2"/>
@@ -4166,7 +4152,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B103" s="6">
         <v>1194084</v>
@@ -4175,7 +4161,7 @@
         <v>111</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E103" t="b">
         <f t="shared" si="2"/>
@@ -4188,7 +4174,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B104" s="4">
         <v>707871</v>
@@ -4197,7 +4183,7 @@
         <v>125</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E104" t="b">
         <f t="shared" si="2"/>
@@ -4210,7 +4196,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B105" s="6">
         <v>1621769</v>
@@ -4219,7 +4205,7 @@
         <v>101</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E105" t="b">
         <f t="shared" si="2"/>
@@ -4232,7 +4218,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B106" s="4">
         <v>2535918</v>
@@ -4241,7 +4227,7 @@
         <v>82</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E106" t="b">
         <f t="shared" si="2"/>
@@ -4254,7 +4240,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B107" s="6">
         <v>88602</v>
@@ -4263,7 +4249,7 @@
         <v>170</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E107" t="b">
         <f t="shared" si="2"/>
@@ -4276,7 +4262,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B108" s="4">
         <v>14751</v>
@@ -4285,7 +4271,7 @@
         <v>162</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E108" t="b">
         <f t="shared" si="2"/>
@@ -4298,7 +4284,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B109" s="6">
         <v>1115025</v>
@@ -4307,7 +4293,7 @@
         <v>116</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E109" t="b">
         <f t="shared" si="2"/>
@@ -4320,7 +4306,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B110" s="4">
         <v>32824</v>
@@ -4329,7 +4315,7 @@
         <v>195</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E110" t="b">
         <f t="shared" si="2"/>
@@ -4342,7 +4328,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B111" s="6">
         <v>2397517</v>
@@ -4351,7 +4337,7 @@
         <v>85</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E111" t="b">
         <f t="shared" si="2"/>
@@ -4364,7 +4350,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B112" s="4">
         <v>468348</v>
@@ -4373,7 +4359,7 @@
         <v>132</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E112" t="b">
         <f t="shared" si="2"/>
@@ -4386,7 +4372,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B113" s="6">
         <v>371512</v>
@@ -4395,7 +4381,7 @@
         <v>135</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E113" t="b">
         <f t="shared" si="2"/>
@@ -4408,7 +4394,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B114" s="4">
         <v>1314969</v>
@@ -4417,7 +4403,7 @@
         <v>109</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E114" t="b">
         <f t="shared" si="2"/>
@@ -4430,7 +4416,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B115" s="6">
         <v>452185</v>
@@ -4439,7 +4425,7 @@
         <v>133</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E115" t="b">
         <f t="shared" si="2"/>
@@ -4452,7 +4438,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B116" s="4">
         <v>71015</v>
@@ -4461,7 +4447,7 @@
         <v>124</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E116" t="b">
         <f t="shared" si="2"/>
@@ -4474,7 +4460,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B117" s="6">
         <v>19200408</v>
@@ -4483,7 +4469,7 @@
         <v>26</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E117" t="b">
         <f t="shared" si="2"/>
@@ -4496,7 +4482,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B118" s="4">
         <v>15356</v>
@@ -4505,7 +4491,7 @@
         <v>159</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E118" t="b">
         <f t="shared" si="2"/>
@@ -4518,7 +4504,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B119" s="6">
         <v>336059</v>
@@ -4527,7 +4513,7 @@
         <v>138</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E119" t="b">
         <f t="shared" si="2"/>
@@ -4540,7 +4526,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B120" s="4">
         <v>286885</v>
@@ -4549,7 +4535,7 @@
         <v>142</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E120" t="b">
         <f t="shared" si="2"/>
@@ -4562,7 +4548,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B121" s="6">
         <v>6848</v>
@@ -4571,7 +4557,7 @@
         <v>205</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E121" t="b">
         <f t="shared" si="2"/>
@@ -4584,7 +4570,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B122" s="4">
         <v>180358</v>
@@ -4593,7 +4579,7 @@
         <v>157</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E122" t="b">
         <f t="shared" si="2"/>
@@ -4606,7 +4592,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B123" s="6">
         <v>54355</v>
@@ -4615,7 +4601,7 @@
         <v>129</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E123" t="b">
         <f t="shared" si="2"/>
@@ -4628,7 +4614,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B124" s="4">
         <v>44173551</v>
@@ -4637,7 +4623,7 @@
         <v>11</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E124" t="b">
         <f t="shared" si="2"/>
@@ -4650,7 +4636,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B125" s="6">
         <v>27659</v>
@@ -4659,7 +4645,7 @@
         <v>196</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E125" t="b">
         <f t="shared" si="2"/>
@@ -4672,7 +4658,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B126" s="4">
         <v>1585973</v>
@@ -4681,7 +4667,7 @@
         <v>103</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E126" t="b">
         <f t="shared" si="2"/>
@@ -4694,7 +4680,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B127" s="6">
         <v>26544</v>
@@ -4703,7 +4689,7 @@
         <v>198</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E127" t="b">
         <f t="shared" si="2"/>
@@ -4716,7 +4702,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B128" s="4">
         <v>52152</v>
@@ -4725,7 +4711,7 @@
         <v>131</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E128" t="b">
         <f t="shared" si="2"/>
@@ -4738,7 +4724,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B129" s="6">
         <v>373655</v>
@@ -4747,7 +4733,7 @@
         <v>134</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E129" t="b">
         <f t="shared" si="2"/>
@@ -4760,7 +4746,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B130" s="4">
         <v>1583</v>
@@ -4769,7 +4755,7 @@
         <v>209</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E130" t="b">
         <f t="shared" si="2"/>
@@ -4782,7 +4768,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B131" s="6">
         <v>17770081</v>
@@ -4791,7 +4777,7 @@
         <v>30</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E131" t="b">
         <f t="shared" ref="E131:E194" si="4">B131&gt;1000000</f>
@@ -4804,7 +4790,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B132" s="4">
         <v>1140311</v>
@@ -4813,7 +4799,7 @@
         <v>114</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E132" t="b">
         <f t="shared" si="4"/>
@@ -4826,7 +4812,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B133" s="6">
         <v>280288</v>
@@ -4835,7 +4821,7 @@
         <v>143</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E133" t="b">
         <f t="shared" si="4"/>
@@ -4848,7 +4834,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B134" s="4">
         <v>3332602</v>
@@ -4857,7 +4843,7 @@
         <v>77</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E134" t="b">
         <f t="shared" si="4"/>
@@ -4870,7 +4856,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B135" s="6">
         <v>15559488</v>
@@ -4879,7 +4865,7 @@
         <v>32</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E135" t="b">
         <f t="shared" si="4"/>
@@ -4892,7 +4878,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B136" s="4">
         <v>150896</v>
@@ -4901,7 +4887,7 @@
         <v>161</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E136" t="b">
         <f t="shared" si="4"/>
@@ -4914,7 +4900,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B137" s="6">
         <v>3873982</v>
@@ -4923,7 +4909,7 @@
         <v>73</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E137" t="b">
         <f t="shared" si="4"/>
@@ -4936,7 +4922,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B138" s="4">
         <v>77324</v>
@@ -4945,7 +4931,7 @@
         <v>121</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E138" t="b">
         <f t="shared" si="4"/>
@@ -4958,7 +4944,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B139" s="6">
         <v>230084</v>
@@ -4967,7 +4953,7 @@
         <v>150</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E139" t="b">
         <f t="shared" si="4"/>
@@ -4980,7 +4966,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B140" s="4">
         <v>55930391</v>
@@ -4989,7 +4975,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E140" t="b">
         <f t="shared" si="4"/>
@@ -5002,7 +4988,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B141" s="6">
         <v>1011</v>
@@ -5011,7 +4997,7 @@
         <v>211</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E141" t="b">
         <f t="shared" si="4"/>
@@ -5024,7 +5010,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B142" s="4">
         <v>4471907</v>
@@ -5033,7 +5019,7 @@
         <v>65</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E142" t="b">
         <f t="shared" si="4"/>
@@ -5046,7 +5032,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B143" s="6">
         <v>1854090</v>
@@ -5055,7 +5041,7 @@
         <v>94</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E143" t="b">
         <f t="shared" si="4"/>
@@ -5068,7 +5054,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B144" s="4">
         <v>18960037</v>
@@ -5077,7 +5063,7 @@
         <v>27</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E144" t="b">
         <f t="shared" si="4"/>
@@ -5090,7 +5076,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B145" s="6">
         <v>1779915</v>
@@ -5099,7 +5085,7 @@
         <v>96</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E145" t="b">
         <f t="shared" si="4"/>
@@ -5112,7 +5098,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B146" s="4">
         <v>1586537</v>
@@ -5121,7 +5107,7 @@
         <v>102</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E146" t="b">
         <f t="shared" si="4"/>
@@ -5134,7 +5120,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B147" s="6">
         <v>145256</v>
@@ -5143,7 +5129,7 @@
         <v>163</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E147" t="b">
         <f t="shared" si="4"/>
@@ -5156,7 +5142,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B148" s="4">
         <v>1771188</v>
@@ -5165,7 +5151,7 @@
         <v>97</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E148" t="b">
         <f t="shared" si="4"/>
@@ -5178,7 +5164,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B149" s="6">
         <v>11287915</v>
@@ -5187,7 +5173,7 @@
         <v>37</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E149" t="b">
         <f t="shared" si="4"/>
@@ -5200,7 +5186,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B150" s="4">
         <v>37602976</v>
@@ -5209,7 +5195,7 @@
         <v>14</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E150" t="b">
         <f t="shared" si="4"/>
@@ -5222,7 +5208,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B151" s="6">
         <v>24969935</v>
@@ -5231,7 +5217,7 @@
         <v>21</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E151" t="b">
         <f t="shared" si="4"/>
@@ -5244,7 +5230,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B152" s="4">
         <v>6900134</v>
@@ -5253,7 +5239,7 @@
         <v>48</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E152" t="b">
         <f t="shared" si="4"/>
@@ -5266,7 +5252,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B153" s="6">
         <v>1897555</v>
@@ -5275,7 +5261,7 @@
         <v>92</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E153" t="b">
         <f t="shared" si="4"/>
@@ -5288,7 +5274,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B154" s="4">
         <v>1719437</v>
@@ -5297,7 +5283,7 @@
         <v>98</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E154" t="b">
         <f t="shared" si="4"/>
@@ -5310,7 +5296,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B155" s="6">
         <v>266635</v>
@@ -5319,7 +5305,7 @@
         <v>145</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E155" t="b">
         <f t="shared" si="4"/>
@@ -5332,7 +5318,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B156" s="4">
         <v>10924252</v>
@@ -5341,7 +5327,7 @@
         <v>38</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E156" t="b">
         <f t="shared" si="4"/>
@@ -5354,7 +5340,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B157" s="6">
         <v>75926004</v>
@@ -5363,7 +5349,7 @@
         <v>6</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E157" t="b">
         <f t="shared" si="4"/>
@@ -5376,7 +5362,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B158" s="4">
         <v>937964</v>
@@ -5385,7 +5371,7 @@
         <v>120</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E158" t="b">
         <f t="shared" si="4"/>
@@ -5398,7 +5384,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B159" s="6">
         <v>2906</v>
@@ -5407,7 +5393,7 @@
         <v>207</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E159" t="b">
         <f t="shared" si="4"/>
@@ -5420,7 +5406,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B160" s="4">
         <v>40251</v>
@@ -5429,7 +5415,7 @@
         <v>189</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E160" t="b">
         <f t="shared" si="4"/>
@@ -5442,7 +5428,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B161" s="6">
         <v>78864</v>
@@ -5451,7 +5437,7 @@
         <v>173</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E161" t="b">
         <f t="shared" si="4"/>
@@ -5464,7 +5450,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B162" s="4">
         <v>49201</v>
@@ -5473,7 +5459,7 @@
         <v>179</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E162" t="b">
         <f t="shared" si="4"/>
@@ -5486,7 +5472,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B163" s="6">
         <v>25111</v>
@@ -5495,7 +5481,7 @@
         <v>199</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E163" t="b">
         <f t="shared" si="4"/>
@@ -5508,7 +5494,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B164" s="4">
         <v>16354</v>
@@ -5517,7 +5503,7 @@
         <v>201</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E164" t="b">
         <f t="shared" si="4"/>
@@ -5530,7 +5516,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B165" s="6">
         <v>39515</v>
@@ -5539,7 +5525,7 @@
         <v>190</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E165" t="b">
         <f t="shared" si="4"/>
@@ -5552,7 +5538,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B166" s="4">
         <v>14328632</v>
@@ -5561,7 +5547,7 @@
         <v>34</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E166" t="b">
         <f t="shared" si="4"/>
@@ -5574,7 +5560,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B167" s="6">
         <v>2490631</v>
@@ -5583,7 +5569,7 @@
         <v>84</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E167" t="b">
         <f t="shared" si="4"/>
@@ -5596,7 +5582,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B168" s="4">
         <v>3500047</v>
@@ -5605,7 +5591,7 @@
         <v>76</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E168" t="b">
         <f t="shared" si="4"/>
@@ -5618,7 +5604,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B169" s="6">
         <v>4238</v>
@@ -5627,7 +5613,7 @@
         <v>185</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E169" t="b">
         <f t="shared" si="4"/>
@@ -5640,7 +5626,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B170" s="4">
         <v>71318</v>
@@ -5649,7 +5635,7 @@
         <v>176</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E170" t="b">
         <f t="shared" si="4"/>
@@ -5662,7 +5648,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B171" s="6">
         <v>3971318</v>
@@ -5671,7 +5657,7 @@
         <v>70</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E171" t="b">
         <f t="shared" si="4"/>
@@ -5684,7 +5670,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B172" s="4">
         <v>4386470</v>
@@ -5693,7 +5679,7 @@
         <v>67</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E172" t="b">
         <f t="shared" si="4"/>
@@ -5706,7 +5692,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B173" s="6">
         <v>1397632</v>
@@ -5715,7 +5701,7 @@
         <v>106</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E173" t="b">
         <f t="shared" si="4"/>
@@ -5728,7 +5714,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B174" s="4">
         <v>40905</v>
@@ -5737,7 +5723,7 @@
         <v>187</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E174" t="b">
         <f t="shared" si="4"/>
@@ -5750,7 +5736,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B175" s="6">
         <v>138849</v>
@@ -5759,7 +5745,7 @@
         <v>165</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E175" t="b">
         <f t="shared" si="4"/>
@@ -5772,7 +5758,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B176" s="4">
         <v>20012275</v>
@@ -5781,7 +5767,7 @@
         <v>25</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E176" t="b">
         <f t="shared" si="4"/>
@@ -5794,7 +5780,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B177" s="6">
         <v>41091681</v>
@@ -5803,7 +5789,7 @@
         <v>12</v>
       </c>
       <c r="D177" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E177" t="b">
         <f t="shared" si="4"/>
@@ -5816,7 +5802,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B178" s="4">
         <v>33870948</v>
@@ -5825,7 +5811,7 @@
         <v>19</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E178" t="b">
         <f t="shared" si="4"/>
@@ -5838,7 +5824,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B179" s="6">
         <v>3927948</v>
@@ -5847,7 +5833,7 @@
         <v>71</v>
       </c>
       <c r="D179" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E179" t="b">
         <f t="shared" si="4"/>
@@ -5860,7 +5846,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B180" s="4">
         <v>7183409</v>
@@ -5869,7 +5855,7 @@
         <v>46</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E180" t="b">
         <f t="shared" si="4"/>
@@ -5882,7 +5868,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B181" s="6">
         <v>194269</v>
@@ -5891,7 +5877,7 @@
         <v>154</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E181" t="b">
         <f t="shared" si="4"/>
@@ -5904,7 +5890,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B182" s="4">
         <v>288225</v>
@@ -5913,7 +5899,7 @@
         <v>141</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E182" t="b">
         <f t="shared" si="4"/>
@@ -5926,7 +5912,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B183" s="6">
         <v>8557561</v>
@@ -5935,7 +5921,7 @@
         <v>44</v>
       </c>
       <c r="D183" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E183" t="b">
         <f t="shared" si="4"/>
@@ -5948,7 +5934,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B184" s="4">
         <v>6752540</v>
@@ -5957,7 +5943,7 @@
         <v>49</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E184" t="b">
         <f t="shared" si="4"/>
@@ -5970,7 +5956,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B185" s="6">
         <v>5474994</v>
@@ -5979,7 +5965,7 @@
         <v>55</v>
       </c>
       <c r="D185" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E185" t="b">
         <f t="shared" si="4"/>
@@ -5992,7 +5978,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B186" s="4">
         <v>17656414</v>
@@ -6001,7 +5987,7 @@
         <v>31</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E186" t="b">
         <f t="shared" si="4"/>
@@ -6014,7 +6000,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B187" s="6">
         <v>1127193</v>
@@ -6023,7 +6009,7 @@
         <v>115</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E187" t="b">
         <f t="shared" si="4"/>
@@ -6036,7 +6022,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B188" s="4">
         <v>6136331</v>
@@ -6045,7 +6031,7 @@
         <v>51</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E188" t="b">
         <f t="shared" si="4"/>
@@ -6058,7 +6044,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B189" s="6">
         <v>17779139</v>
@@ -6067,7 +6053,7 @@
         <v>29</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E189" t="b">
         <f t="shared" si="4"/>
@@ -6080,7 +6066,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B190" s="4">
         <v>226855</v>
@@ -6089,7 +6075,7 @@
         <v>152</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E190" t="b">
         <f t="shared" si="4"/>
@@ -6102,7 +6088,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B191" s="6">
         <v>229122</v>
@@ -6111,7 +6097,7 @@
         <v>151</v>
       </c>
       <c r="D191" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E191" t="b">
         <f t="shared" si="4"/>
@@ -6124,7 +6110,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B192" s="4">
         <v>278442</v>
@@ -6133,7 +6119,7 @@
         <v>144</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E192" t="b">
         <f t="shared" si="4"/>
@@ -6146,7 +6132,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B193" s="6">
         <v>37003</v>
@@ -6155,7 +6141,7 @@
         <v>194</v>
       </c>
       <c r="D193" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E193" t="b">
         <f t="shared" si="4"/>
@@ -6168,7 +6154,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B194" s="4">
         <v>729897</v>
@@ -6177,7 +6163,7 @@
         <v>123</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E194" t="b">
         <f t="shared" si="4"/>
@@ -6190,7 +6176,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B195" s="6">
         <v>4447885</v>
@@ -6199,7 +6185,7 @@
         <v>66</v>
       </c>
       <c r="D195" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E195" t="b">
         <f t="shared" ref="E195:E213" si="6">B195&gt;1000000</f>
@@ -6212,7 +6198,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B196" s="4">
         <v>35990932</v>
@@ -6221,7 +6207,7 @@
         <v>17</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E196" t="b">
         <f t="shared" si="6"/>
@@ -6234,7 +6220,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B197" s="6">
         <v>363735</v>
@@ -6243,7 +6229,7 @@
         <v>137</v>
       </c>
       <c r="D197" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E197" t="b">
         <f t="shared" si="6"/>
@@ -6256,7 +6242,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B198" s="4">
         <v>3717</v>
@@ -6265,7 +6251,7 @@
         <v>206</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E198" t="b">
         <f t="shared" si="6"/>
@@ -6278,7 +6264,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B199" s="6">
         <v>42687</v>
@@ -6287,7 +6273,7 @@
         <v>184</v>
       </c>
       <c r="D199" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E199" t="b">
         <f t="shared" si="6"/>
@@ -6300,7 +6286,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B200" s="4">
         <v>4941704</v>
@@ -6309,7 +6295,7 @@
         <v>60</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E200" t="b">
         <f t="shared" si="6"/>
@@ -6322,7 +6308,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B201" s="6">
         <v>15115820</v>
@@ -6331,7 +6317,7 @@
         <v>33</v>
       </c>
       <c r="D201" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E201" t="b">
         <f t="shared" si="6"/>
@@ -6344,7 +6330,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B202" s="4">
         <v>4517169</v>
@@ -6353,7 +6339,7 @@
         <v>64</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E202" t="b">
         <f t="shared" si="6"/>
@@ -6366,7 +6352,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B203" s="6">
         <v>54861245</v>
@@ -6375,7 +6361,7 @@
         <v>9</v>
       </c>
       <c r="D203" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E203" t="b">
         <f t="shared" si="6"/>
@@ -6388,7 +6374,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B204" s="4">
         <v>254295536</v>
@@ -6397,7 +6383,7 @@
         <v>2</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E204" t="b">
         <f t="shared" si="6"/>
@@ -6410,7 +6396,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B205" s="6">
         <v>1827781</v>
@@ -6419,7 +6405,7 @@
         <v>95</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E205" t="b">
         <f t="shared" si="6"/>
@@ -6432,7 +6418,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B206" s="4">
         <v>10369924</v>
@@ -6441,7 +6427,7 @@
         <v>40</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E206" t="b">
         <f t="shared" si="6"/>
@@ -6454,7 +6440,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B207" s="6">
         <v>1383</v>
@@ -6476,7 +6462,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B208" s="4">
         <v>27147</v>
@@ -6485,7 +6471,7 @@
         <v>197</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E208" t="b">
         <f t="shared" si="6"/>
@@ -6498,7 +6484,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B209" s="6">
         <v>12353883</v>
@@ -6507,7 +6493,7 @@
         <v>36</v>
       </c>
       <c r="D209" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E209" t="b">
         <f t="shared" si="6"/>
@@ -6520,7 +6506,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B210" s="4">
         <v>36140967</v>
@@ -6529,7 +6515,7 @@
         <v>16</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E210" t="b">
         <f t="shared" si="6"/>
@@ -6542,7 +6528,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B211" s="6">
         <v>4321814</v>
@@ -6551,7 +6537,7 @@
         <v>68</v>
       </c>
       <c r="D211" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E211" t="b">
         <f t="shared" si="6"/>
@@ -6564,7 +6550,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B212" s="4">
         <v>1860966</v>
@@ -6573,7 +6559,7 @@
         <v>93</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E212" t="b">
         <f t="shared" si="6"/>
@@ -6586,7 +6572,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B213" s="8">
         <v>2156791</v>
@@ -6595,7 +6581,7 @@
         <v>89</v>
       </c>
       <c r="D213" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E213" t="b">
         <f t="shared" si="6"/>

</xml_diff>